<commit_message>
change covid 54 new2
</commit_message>
<xml_diff>
--- a/help/54_COVID_19_new2.xlsx
+++ b/help/54_COVID_19_new2.xlsx
@@ -142,9 +142,6 @@
     <t>Остатки неиспользованных тест-систем</t>
   </si>
   <si>
-    <t>С нрастающим итогом</t>
-  </si>
-  <si>
     <t>за сутки</t>
   </si>
   <si>
@@ -155,6 +152,9 @@
   </si>
   <si>
     <t>Охват тестирования населения на Covid-19 методом ИХА (экспресс-тест)</t>
+  </si>
+  <si>
+    <t>С нарастающим итогом</t>
   </si>
 </sst>
 </file>
@@ -590,7 +590,7 @@
   <dimension ref="B1:J248"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -606,7 +606,7 @@
     <row r="1" spans="2:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:10" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
@@ -631,11 +631,11 @@
         <v>38</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G3" s="9"/>
       <c r="H3" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I3" s="9"/>
       <c r="J3" s="10" t="s">
@@ -648,16 +648,16 @@
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
       <c r="F4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="G4" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="G4" s="4" t="s">
-        <v>41</v>
-      </c>
       <c r="H4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="I4" s="4" t="s">
         <v>40</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>41</v>
       </c>
       <c r="J4" s="11"/>
     </row>

</xml_diff>